<commit_message>
more figures and added data
</commit_message>
<xml_diff>
--- a/data/TWP emission data_IDIADA_v01_andSIML.xlsx
+++ b/data/TWP emission data_IDIADA_v01_andSIML.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rivmnl-my.sharepoint.com/personal/joris_quik_rivm_nl/Documents/Git projects/tyre-friction-abrassion-emission_2024/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quikj\rivm.nl\LEON-Tyres - WP3 Microplastics\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{6040C974-9C03-462F-91D7-96FE4AC2DD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C24C227D-CEAA-4DD2-8D2A-6F442FB3D245}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881749E5-F2BB-4584-8094-F28CF42164A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1B08EC6D-E4F6-452D-BA0B-C8BBC214CF8F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="9" xr2:uid="{1B08EC6D-E4F6-452D-BA0B-C8BBC214CF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="8" r:id="rId1"/>
@@ -19,16 +19,23 @@
     <sheet name="Maneuver data" sheetId="1" r:id="rId4"/>
     <sheet name="Vehicle data" sheetId="3" r:id="rId5"/>
     <sheet name="Tyre_data" sheetId="4" r:id="rId6"/>
-    <sheet name="Abrasion" sheetId="11" r:id="rId7"/>
-    <sheet name="Tyre_ADAC" sheetId="13" r:id="rId8"/>
-    <sheet name="Abrasion_ADAC" sheetId="12" r:id="rId9"/>
-    <sheet name="Constants" sheetId="5" r:id="rId10"/>
-    <sheet name="Label fuel efficiency class" sheetId="6" state="hidden" r:id="rId11"/>
-    <sheet name="Label wet grip class" sheetId="7" state="hidden" r:id="rId12"/>
+    <sheet name="Constants" sheetId="5" r:id="rId7"/>
+    <sheet name="Abrasion" sheetId="11" r:id="rId8"/>
+    <sheet name="Cenek et al. 1997" sheetId="14" r:id="rId9"/>
+    <sheet name="Abrasion_ADAC" sheetId="12" r:id="rId10"/>
+    <sheet name="Tyre_ADAC" sheetId="13" r:id="rId11"/>
+    <sheet name="Label fuel efficiency class" sheetId="6" state="hidden" r:id="rId12"/>
+    <sheet name="Label wet grip class" sheetId="7" state="hidden" r:id="rId13"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId13"/>
+    <externalReference r:id="rId14"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Abrasion_ADAC!$B$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Abrasion_ADAC!$B$2:$B$16</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Abrasion_ADAC!$B$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Abrasion_ADAC!$B$2:$B$16</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -228,6 +235,51 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={5C32FB0E-B292-4226-A4D7-0FC189658EDC}</author>
+    <author>tc={F847441E-647B-4A01-89C5-91E38E7644E4}</author>
+    <author>tc={F0920C63-E50A-4591-A7F2-970D431E17A9}</author>
+    <author>tc={2567C819-AF5D-4925-828A-E46A4F184DA4}</author>
+  </authors>
+  <commentList>
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{5C32FB0E-B292-4226-A4D7-0FC189658EDC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    TWO labels *AB or BB</t>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="1" shapeId="0" xr:uid="{F847441E-647B-4A01-89C5-91E38E7644E4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Niet in EPREL data base (label van ADAC site) https://www.adac.de/rund-ums-fahrzeug/ausstattung-technik-zubehoer/reifen/reifentest/sommerreifen/205-55-r16/king-meiler-sport-1-id-4476/</t>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="2" shapeId="0" xr:uid="{F0920C63-E50A-4591-A7F2-970D431E17A9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Premitra 5 niet terug te vinden, gebruik label van HP5 model</t>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="3" shapeId="0" xr:uid="{2567C819-AF5D-4925-828A-E46A4F184DA4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Many different ones with raning (also other brands, different on martket dates). Used 40605 label</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>tc={74A80BAF-D6C7-46BC-B829-ED1B8A239F99}</author>
     <author>tc={0D79CBC1-2634-45C8-9083-88EF78337D3C}</author>
     <author>tc={6C100F98-F6FB-45F9-87E2-D6113A56C424}</author>
@@ -270,53 +322,8 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={5C32FB0E-B292-4226-A4D7-0FC189658EDC}</author>
-    <author>tc={F847441E-647B-4A01-89C5-91E38E7644E4}</author>
-    <author>tc={F0920C63-E50A-4591-A7F2-970D431E17A9}</author>
-    <author>tc={2567C819-AF5D-4925-828A-E46A4F184DA4}</author>
-  </authors>
-  <commentList>
-    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{5C32FB0E-B292-4226-A4D7-0FC189658EDC}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    TWO labels *AB or BB</t>
-      </text>
-    </comment>
-    <comment ref="A9" authorId="1" shapeId="0" xr:uid="{F847441E-647B-4A01-89C5-91E38E7644E4}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Niet in EPREL data base (label van ADAC site) https://www.adac.de/rund-ums-fahrzeug/ausstattung-technik-zubehoer/reifen/reifentest/sommerreifen/205-55-r16/king-meiler-sport-1-id-4476/</t>
-      </text>
-    </comment>
-    <comment ref="A12" authorId="2" shapeId="0" xr:uid="{F0920C63-E50A-4591-A7F2-970D431E17A9}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Premitra 5 niet terug te vinden, gebruik label van HP5 model</t>
-      </text>
-    </comment>
-    <comment ref="A15" authorId="3" shapeId="0" xr:uid="{2567C819-AF5D-4925-828A-E46A4F184DA4}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Many different ones with raning (also other brands, different on martket dates). Used 40605 label</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="406">
   <si>
     <t>This is a spreadsheet collecting all the data needed to apply the tyre friction abrasion model.</t>
   </si>
@@ -1323,12 +1330,6 @@
     <t>Volkswagen</t>
   </si>
   <si>
-    <t>Tyre name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADAC wear g per 1000 km </t>
-  </si>
-  <si>
     <t xml:space="preserve">Goodyear Efficient Grip Performance 2 </t>
   </si>
   <si>
@@ -1513,6 +1514,33 @@
   </si>
   <si>
     <t>MMoWStr4</t>
+  </si>
+  <si>
+    <t>Abrasion rate (mg/km)</t>
+  </si>
+  <si>
+    <t>Tyre</t>
+  </si>
+  <si>
+    <t>Abr. Rate dry (g/km)</t>
+  </si>
+  <si>
+    <t>Abr. Rate. dm^3 / 1000km</t>
+  </si>
+  <si>
+    <t>CT (dm^3 /MJ)</t>
+  </si>
+  <si>
+    <t>tyre wear density g /dm^3</t>
+  </si>
+  <si>
+    <t>abrasion coefficient (g / MJ)</t>
+  </si>
+  <si>
+    <t>abrasion coefficient (mg / KJ)</t>
+  </si>
+  <si>
+    <t>Friction per km (kJ/km)</t>
   </si>
 </sst>
 </file>
@@ -1524,7 +1552,7 @@
     <numFmt numFmtId="165" formatCode="&quot;\&quot;#,##0.00;[Red]&quot;\&quot;\-#,##0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1569,6 +1597,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1836,7 +1871,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1894,6 +1929,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1949,6 +1985,657 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.3</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{8C34953D-F100-4CEF-B70A-5C3E49BCC665}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:v>Abrasion rate (mg/km)</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1"/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>ADAC Test 2021</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>ADAC Test 2021</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling min="60"/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Abrasion rate (mg/km)</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Abrasion rate (mg/km)</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/documenttasks/documenttask1.xml><?xml version="1.0" encoding="utf-8"?>
 <Tasks xmlns="http://schemas.microsoft.com/office/tasks/2019/documenttasks">
   <Task id="{5D13ECFB-BB48-4CF3-90B8-66FDCD19F7E3}">
@@ -1980,6 +2667,138 @@
     </History>
   </Task>
 </Tasks>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>488950</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>32344</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>43233</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{317C9391-1E62-4CD6-ACC4-B65E7C4D16D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5975350" y="120650"/>
+          <a:ext cx="6858594" cy="3517953"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="Chart 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D87683CC-5C0B-9DA2-9759-D78797276A59}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3733800" y="323850"/>
+              <a:ext cx="2164080" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2400,6 +3219,23 @@
 
 <file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A8" dT="2023-06-16T12:48:08.77" personId="{E04D0CC9-932F-4577-9D81-3BA1E2CD2B36}" id="{5C32FB0E-B292-4226-A4D7-0FC189658EDC}">
+    <text>TWO labels *AB or BB</text>
+  </threadedComment>
+  <threadedComment ref="A9" dT="2023-06-16T12:51:46.08" personId="{E04D0CC9-932F-4577-9D81-3BA1E2CD2B36}" id="{F847441E-647B-4A01-89C5-91E38E7644E4}">
+    <text>Niet in EPREL data base (label van ADAC site) https://www.adac.de/rund-ums-fahrzeug/ausstattung-technik-zubehoer/reifen/reifentest/sommerreifen/205-55-r16/king-meiler-sport-1-id-4476/</text>
+  </threadedComment>
+  <threadedComment ref="A12" dT="2023-06-16T12:57:18.32" personId="{E04D0CC9-932F-4577-9D81-3BA1E2CD2B36}" id="{F0920C63-E50A-4591-A7F2-970D431E17A9}">
+    <text>Premitra 5 niet terug te vinden, gebruik label van HP5 model</text>
+  </threadedComment>
+  <threadedComment ref="A15" dT="2023-06-16T13:03:23.81" personId="{E04D0CC9-932F-4577-9D81-3BA1E2CD2B36}" id="{2567C819-AF5D-4925-828A-E46A4F184DA4}">
+    <text>Many different ones with raning (also other brands, different on martket dates). Used 40605 label</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="B8" dT="2023-06-16T12:48:08.77" personId="{E04D0CC9-932F-4577-9D81-3BA1E2CD2B36}" id="{74A80BAF-D6C7-46BC-B829-ED1B8A239F99}">
     <text>TWO labels *AB or BB</text>
   </threadedComment>
@@ -2410,23 +3246,6 @@
     <text>Premitra 5 niet terug te vinden, gebruik label van HP5 model</text>
   </threadedComment>
   <threadedComment ref="B15" dT="2023-06-16T13:03:23.81" personId="{E04D0CC9-932F-4577-9D81-3BA1E2CD2B36}" id="{7C540CA7-1742-41AA-8C18-2D835D3B4F82}">
-    <text>Many different ones with raning (also other brands, different on martket dates). Used 40605 label</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
-<file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A8" dT="2023-06-16T12:48:08.77" personId="{E04D0CC9-932F-4577-9D81-3BA1E2CD2B36}" id="{5C32FB0E-B292-4226-A4D7-0FC189658EDC}">
-    <text>TWO labels *AB or BB</text>
-  </threadedComment>
-  <threadedComment ref="A9" dT="2023-06-16T12:51:46.08" personId="{E04D0CC9-932F-4577-9D81-3BA1E2CD2B36}" id="{F847441E-647B-4A01-89C5-91E38E7644E4}">
-    <text>Niet in EPREL data base (label van ADAC site) https://www.adac.de/rund-ums-fahrzeug/ausstattung-technik-zubehoer/reifen/reifentest/sommerreifen/205-55-r16/king-meiler-sport-1-id-4476/</text>
-  </threadedComment>
-  <threadedComment ref="A12" dT="2023-06-16T12:57:18.32" personId="{E04D0CC9-932F-4577-9D81-3BA1E2CD2B36}" id="{F0920C63-E50A-4591-A7F2-970D431E17A9}">
-    <text>Premitra 5 niet terug te vinden, gebruik label van HP5 model</text>
-  </threadedComment>
-  <threadedComment ref="A15" dT="2023-06-16T13:03:23.81" personId="{E04D0CC9-932F-4577-9D81-3BA1E2CD2B36}" id="{2567C819-AF5D-4925-828A-E46A4F184DA4}">
     <text>Many different ones with raning (also other brands, different on martket dates). Used 40605 label</text>
   </threadedComment>
 </ThreadedComments>
@@ -2515,10 +3334,10 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="10" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -2528,199 +3347,538 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E0172C-DF0F-4DBA-8FF0-B64EC2D7369B}">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33AA0F0-47E1-4AC0-A88E-CD4E07267161}">
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.5546875" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>295</v>
+        <v>398</v>
       </c>
       <c r="B1" t="s">
-        <v>296</v>
-      </c>
-      <c r="C1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>300</v>
-      </c>
-      <c r="B2" t="s">
-        <v>301</v>
-      </c>
-      <c r="C2">
-        <v>9.81</v>
-      </c>
-      <c r="D2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>335</v>
+      </c>
+      <c r="B2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>303</v>
-      </c>
-      <c r="B3" t="s">
-        <v>304</v>
-      </c>
-      <c r="C3">
-        <v>0.85</v>
-      </c>
-      <c r="D3" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>336</v>
+      </c>
+      <c r="B3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>306</v>
-      </c>
-      <c r="B4" t="s">
-        <v>307</v>
-      </c>
-      <c r="C4">
-        <v>0.13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>337</v>
+      </c>
+      <c r="B4">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>308</v>
-      </c>
-      <c r="B5" t="s">
-        <v>309</v>
-      </c>
-      <c r="C5">
-        <v>0.15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>338</v>
+      </c>
+      <c r="B5">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>310</v>
-      </c>
-      <c r="B6" t="s">
-        <v>311</v>
-      </c>
-      <c r="C6">
-        <v>1.2050000000000001</v>
-      </c>
-      <c r="D6" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>339</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>313</v>
-      </c>
-      <c r="B7" t="s">
-        <v>314</v>
-      </c>
-      <c r="C7">
-        <v>1.07</v>
-      </c>
-      <c r="D7" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>340</v>
+      </c>
+      <c r="B7">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>315</v>
-      </c>
-      <c r="B8" t="s">
-        <v>316</v>
-      </c>
-      <c r="C8">
-        <v>1.47</v>
-      </c>
-      <c r="D8" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>341</v>
+      </c>
+      <c r="B8">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>317</v>
-      </c>
-      <c r="B9" t="s">
-        <v>318</v>
-      </c>
-      <c r="C9">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>342</v>
+      </c>
+      <c r="B9">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>319</v>
-      </c>
-      <c r="B10" t="s">
-        <v>318</v>
-      </c>
-      <c r="C10">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>343</v>
+      </c>
+      <c r="B10">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>320</v>
-      </c>
-      <c r="B11" t="s">
-        <v>318</v>
-      </c>
-      <c r="C11">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>344</v>
+      </c>
+      <c r="B11">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>321</v>
-      </c>
-      <c r="B12" t="s">
-        <v>318</v>
-      </c>
-      <c r="C12">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>345</v>
+      </c>
+      <c r="B12">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>322</v>
-      </c>
-      <c r="B13" t="s">
-        <v>323</v>
-      </c>
-      <c r="C13">
-        <v>0.68</v>
-      </c>
-      <c r="D13" t="s">
-        <v>324</v>
+        <v>346</v>
+      </c>
+      <c r="B13">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>347</v>
+      </c>
+      <c r="B14">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>348</v>
+      </c>
+      <c r="B15">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>349</v>
+      </c>
+      <c r="B16">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B7D490-4724-44DB-9756-35EF11163C36}">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C2" t="s">
+        <v>352</v>
+      </c>
+      <c r="D2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E3" t="s">
+        <v>248</v>
+      </c>
+      <c r="F3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>368</v>
+      </c>
+      <c r="B4" t="s">
+        <v>337</v>
+      </c>
+      <c r="C4" t="s">
+        <v>354</v>
+      </c>
+      <c r="D4" t="s">
+        <v>247</v>
+      </c>
+      <c r="E4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F4" t="s">
+        <v>229</v>
+      </c>
+      <c r="G4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>369</v>
+      </c>
+      <c r="B5" t="s">
+        <v>338</v>
+      </c>
+      <c r="C5" t="s">
+        <v>355</v>
+      </c>
+      <c r="D5" t="s">
+        <v>247</v>
+      </c>
+      <c r="E5" t="s">
+        <v>248</v>
+      </c>
+      <c r="F5" t="s">
+        <v>229</v>
+      </c>
+      <c r="G5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>370</v>
+      </c>
+      <c r="B6" t="s">
+        <v>339</v>
+      </c>
+      <c r="C6" t="s">
+        <v>356</v>
+      </c>
+      <c r="D6" t="s">
+        <v>247</v>
+      </c>
+      <c r="E6" t="s">
+        <v>247</v>
+      </c>
+      <c r="F6" t="s">
+        <v>229</v>
+      </c>
+      <c r="G6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>379</v>
+      </c>
+      <c r="B7" t="s">
+        <v>340</v>
+      </c>
+      <c r="C7" t="s">
+        <v>357</v>
+      </c>
+      <c r="D7" t="s">
+        <v>247</v>
+      </c>
+      <c r="E7" t="s">
+        <v>242</v>
+      </c>
+      <c r="F7" t="s">
+        <v>229</v>
+      </c>
+      <c r="G7" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>371</v>
+      </c>
+      <c r="B8" t="s">
+        <v>341</v>
+      </c>
+      <c r="C8" t="s">
+        <v>358</v>
+      </c>
+      <c r="D8" t="s">
+        <v>242</v>
+      </c>
+      <c r="E8" t="s">
+        <v>248</v>
+      </c>
+      <c r="F8" t="s">
+        <v>229</v>
+      </c>
+      <c r="G8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B9" t="s">
+        <v>342</v>
+      </c>
+      <c r="C9" t="s">
+        <v>359</v>
+      </c>
+      <c r="D9" t="s">
+        <v>247</v>
+      </c>
+      <c r="E9" t="s">
+        <v>248</v>
+      </c>
+      <c r="F9" t="s">
+        <v>229</v>
+      </c>
+      <c r="G9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B10" t="s">
+        <v>343</v>
+      </c>
+      <c r="C10" t="s">
+        <v>360</v>
+      </c>
+      <c r="D10" t="s">
+        <v>247</v>
+      </c>
+      <c r="E10" t="s">
+        <v>248</v>
+      </c>
+      <c r="F10" t="s">
+        <v>229</v>
+      </c>
+      <c r="G10" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>374</v>
+      </c>
+      <c r="B11" t="s">
+        <v>344</v>
+      </c>
+      <c r="C11" t="s">
+        <v>361</v>
+      </c>
+      <c r="D11" t="s">
+        <v>247</v>
+      </c>
+      <c r="E11" t="s">
+        <v>242</v>
+      </c>
+      <c r="F11" t="s">
+        <v>229</v>
+      </c>
+      <c r="G11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>375</v>
+      </c>
+      <c r="B12" t="s">
+        <v>345</v>
+      </c>
+      <c r="C12" t="s">
+        <v>362</v>
+      </c>
+      <c r="D12" t="s">
+        <v>247</v>
+      </c>
+      <c r="E12" t="s">
+        <v>242</v>
+      </c>
+      <c r="F12" t="s">
+        <v>229</v>
+      </c>
+      <c r="G12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>376</v>
+      </c>
+      <c r="B13" t="s">
+        <v>346</v>
+      </c>
+      <c r="C13" t="s">
+        <v>363</v>
+      </c>
+      <c r="D13" t="s">
+        <v>242</v>
+      </c>
+      <c r="E13" t="s">
+        <v>248</v>
+      </c>
+      <c r="F13" t="s">
+        <v>229</v>
+      </c>
+      <c r="G13" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>377</v>
+      </c>
+      <c r="B14" t="s">
+        <v>347</v>
+      </c>
+      <c r="C14" t="s">
+        <v>364</v>
+      </c>
+      <c r="D14" t="s">
+        <v>247</v>
+      </c>
+      <c r="E14" t="s">
+        <v>242</v>
+      </c>
+      <c r="F14" t="s">
+        <v>229</v>
+      </c>
+      <c r="G14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>252</v>
+      </c>
+      <c r="B15" t="s">
+        <v>348</v>
+      </c>
+      <c r="C15" t="s">
+        <v>365</v>
+      </c>
+      <c r="D15" t="s">
+        <v>248</v>
+      </c>
+      <c r="E15" t="s">
+        <v>248</v>
+      </c>
+      <c r="F15" t="s">
+        <v>229</v>
+      </c>
+      <c r="G15" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>378</v>
+      </c>
+      <c r="B16" t="s">
+        <v>349</v>
+      </c>
+      <c r="C16" t="s">
+        <v>366</v>
+      </c>
+      <c r="D16" t="s">
+        <v>247</v>
+      </c>
+      <c r="E16" t="s">
+        <v>242</v>
+      </c>
+      <c r="F16" t="s">
+        <v>229</v>
+      </c>
+      <c r="G16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F501E61A-82C5-43C3-BC60-CB8CE2E4C1FF}">
   <dimension ref="A1:D31"/>
   <sheetViews>
@@ -3178,7 +4336,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69EBB41-BAEF-40B9-810D-EC61876EF034}">
   <dimension ref="A1:D31"/>
   <sheetViews>
@@ -3640,7 +4798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF35CD9C-6566-45D5-AC37-7D32F90348FC}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -3856,16 +5014,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="32" t="s">
+        <v>382</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>383</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>383</v>
+      </c>
+      <c r="D11" s="32" t="s">
         <v>384</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>385</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>385</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>386</v>
       </c>
       <c r="E11" s="32">
         <v>1</v>
@@ -3877,16 +5035,16 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="29" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E12" s="29">
         <v>1</v>
@@ -3898,16 +5056,16 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="32" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E13" s="32">
         <v>1</v>
@@ -5014,13 +6172,13 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B34" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C34" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D34" s="31">
         <f>2*PI()*G34*H34/360</f>
@@ -5047,13 +6205,13 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B35" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C35" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D35" s="31">
         <f>D34*5</f>
@@ -5093,8 +6251,8 @@
   <dimension ref="A1:L105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A98" sqref="A98:K105"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8792,16 +9950,16 @@
     </row>
     <row r="98" spans="1:11">
       <c r="A98" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B98" s="32" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C98" t="s">
+        <v>391</v>
+      </c>
+      <c r="D98" s="32" t="s">
         <v>393</v>
-      </c>
-      <c r="D98" s="32" t="s">
-        <v>395</v>
       </c>
       <c r="E98" s="32" t="s">
         <v>122</v>
@@ -8827,16 +9985,16 @@
     </row>
     <row r="99" spans="1:11">
       <c r="A99" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B99" s="32" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C99" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D99" s="32" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E99" s="32" t="s">
         <v>118</v>
@@ -8862,16 +10020,16 @@
     </row>
     <row r="100" spans="1:11">
       <c r="A100" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B100" s="32" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C100" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D100" s="32" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E100" s="32" t="s">
         <v>120</v>
@@ -8897,16 +10055,16 @@
     </row>
     <row r="101" spans="1:11">
       <c r="A101" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B101" s="32" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C101" s="32" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D101" s="32" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E101" s="32" t="s">
         <v>120</v>
@@ -8932,16 +10090,16 @@
     </row>
     <row r="102" spans="1:11">
       <c r="A102" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B102" s="32" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C102" t="s">
+        <v>391</v>
+      </c>
+      <c r="D102" s="32" t="s">
         <v>393</v>
-      </c>
-      <c r="D102" s="32" t="s">
-        <v>395</v>
       </c>
       <c r="E102" s="32" t="s">
         <v>120</v>
@@ -8967,16 +10125,16 @@
     </row>
     <row r="103" spans="1:11">
       <c r="A103" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B103" s="32" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C103" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D103" s="32" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E103" s="32" t="s">
         <v>120</v>
@@ -9002,16 +10160,16 @@
     </row>
     <row r="104" spans="1:11">
       <c r="A104" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B104" s="32" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C104" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D104" s="32" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E104" s="32" t="s">
         <v>120</v>
@@ -9037,16 +10195,16 @@
     </row>
     <row r="105" spans="1:11">
       <c r="A105" t="s">
+        <v>384</v>
+      </c>
+      <c r="B105" s="32" t="s">
         <v>386</v>
       </c>
-      <c r="B105" s="32" t="s">
-        <v>388</v>
-      </c>
       <c r="C105" s="32" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D105" s="32" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E105" s="32" t="s">
         <v>120</v>
@@ -9221,10 +10379,10 @@
         <v>334</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D5" s="30">
         <v>1252</v>
@@ -9416,6 +10574,199 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E0172C-DF0F-4DBA-8FF0-B64EC2D7369B}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5546875" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C2">
+        <v>9.81</v>
+      </c>
+      <c r="D2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C3">
+        <v>0.85</v>
+      </c>
+      <c r="D3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>306</v>
+      </c>
+      <c r="B4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C4">
+        <v>0.13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>308</v>
+      </c>
+      <c r="B5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C5">
+        <v>0.15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>310</v>
+      </c>
+      <c r="B6" t="s">
+        <v>311</v>
+      </c>
+      <c r="C6">
+        <v>1.2050000000000001</v>
+      </c>
+      <c r="D6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>313</v>
+      </c>
+      <c r="B7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C7">
+        <v>1.07</v>
+      </c>
+      <c r="D7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>315</v>
+      </c>
+      <c r="B8" t="s">
+        <v>316</v>
+      </c>
+      <c r="C8">
+        <v>1.47</v>
+      </c>
+      <c r="D8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>317</v>
+      </c>
+      <c r="B9" t="s">
+        <v>318</v>
+      </c>
+      <c r="C9">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>319</v>
+      </c>
+      <c r="B10" t="s">
+        <v>318</v>
+      </c>
+      <c r="C10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>320</v>
+      </c>
+      <c r="B11" t="s">
+        <v>318</v>
+      </c>
+      <c r="C11">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>321</v>
+      </c>
+      <c r="B12" t="s">
+        <v>318</v>
+      </c>
+      <c r="C12">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>322</v>
+      </c>
+      <c r="B13" t="s">
+        <v>323</v>
+      </c>
+      <c r="C13">
+        <v>0.68</v>
+      </c>
+      <c r="D13" t="s">
+        <v>324</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE3834D1-938D-47C6-97E6-CD34B424831C}">
   <dimension ref="B2:V67"/>
   <sheetViews>
@@ -9507,27 +10858,27 @@
         <v>265</v>
       </c>
       <c r="C9" s="15"/>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="37" t="s">
         <v>266</v>
       </c>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="37"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="37"/>
-      <c r="S9" s="37"/>
-      <c r="T9" s="37"/>
-      <c r="U9" s="37"/>
-      <c r="V9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="38"/>
+      <c r="T9" s="38"/>
+      <c r="U9" s="38"/>
+      <c r="V9" s="39"/>
     </row>
     <row r="10" spans="2:22">
       <c r="B10" s="26"/>
@@ -9591,7 +10942,7 @@
       </c>
     </row>
     <row r="11" spans="2:22">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="34" t="s">
         <v>255</v>
       </c>
       <c r="C11" s="17" t="s">
@@ -9656,7 +11007,7 @@
       </c>
     </row>
     <row r="12" spans="2:22">
-      <c r="B12" s="34"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="17" t="s">
         <v>287</v>
       </c>
@@ -9719,7 +11070,7 @@
       </c>
     </row>
     <row r="13" spans="2:22">
-      <c r="B13" s="34"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="17" t="s">
         <v>288</v>
       </c>
@@ -9782,7 +11133,7 @@
       </c>
     </row>
     <row r="14" spans="2:22">
-      <c r="B14" s="34"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="17" t="s">
         <v>289</v>
       </c>
@@ -9845,7 +11196,7 @@
       </c>
     </row>
     <row r="15" spans="2:22">
-      <c r="B15" s="34"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="17" t="s">
         <v>290</v>
       </c>
@@ -9924,7 +11275,7 @@
       </c>
     </row>
     <row r="16" spans="2:22">
-      <c r="B16" s="34"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="17" t="s">
         <v>291</v>
       </c>
@@ -9987,7 +11338,7 @@
       </c>
     </row>
     <row r="17" spans="2:22">
-      <c r="B17" s="35"/>
+      <c r="B17" s="36"/>
       <c r="C17" s="17" t="s">
         <v>292</v>
       </c>
@@ -10073,7 +11424,7 @@
       <c r="V18" s="23"/>
     </row>
     <row r="19" spans="2:22">
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="40" t="s">
         <v>293</v>
       </c>
       <c r="C19" s="17" t="s">
@@ -10138,7 +11489,7 @@
       </c>
     </row>
     <row r="20" spans="2:22">
-      <c r="B20" s="40"/>
+      <c r="B20" s="41"/>
       <c r="C20" s="17" t="s">
         <v>287</v>
       </c>
@@ -10201,7 +11552,7 @@
       </c>
     </row>
     <row r="21" spans="2:22">
-      <c r="B21" s="40"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="17" t="s">
         <v>288</v>
       </c>
@@ -10264,7 +11615,7 @@
       </c>
     </row>
     <row r="22" spans="2:22">
-      <c r="B22" s="40"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="17" t="s">
         <v>289</v>
       </c>
@@ -10327,7 +11678,7 @@
       </c>
     </row>
     <row r="23" spans="2:22">
-      <c r="B23" s="40"/>
+      <c r="B23" s="41"/>
       <c r="C23" s="17" t="s">
         <v>290</v>
       </c>
@@ -10406,7 +11757,7 @@
       </c>
     </row>
     <row r="24" spans="2:22">
-      <c r="B24" s="40"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="17" t="s">
         <v>291</v>
       </c>
@@ -10469,7 +11820,7 @@
       </c>
     </row>
     <row r="25" spans="2:22">
-      <c r="B25" s="41"/>
+      <c r="B25" s="42"/>
       <c r="C25" s="17" t="s">
         <v>292</v>
       </c>
@@ -10555,7 +11906,7 @@
       <c r="V26" s="23"/>
     </row>
     <row r="27" spans="2:22">
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="43" t="s">
         <v>294</v>
       </c>
       <c r="C27" s="17" t="s">
@@ -10620,7 +11971,7 @@
       </c>
     </row>
     <row r="28" spans="2:22">
-      <c r="B28" s="43"/>
+      <c r="B28" s="44"/>
       <c r="C28" s="17" t="s">
         <v>287</v>
       </c>
@@ -10683,7 +12034,7 @@
       </c>
     </row>
     <row r="29" spans="2:22">
-      <c r="B29" s="43"/>
+      <c r="B29" s="44"/>
       <c r="C29" s="17" t="s">
         <v>288</v>
       </c>
@@ -10746,7 +12097,7 @@
       </c>
     </row>
     <row r="30" spans="2:22">
-      <c r="B30" s="43"/>
+      <c r="B30" s="44"/>
       <c r="C30" s="17" t="s">
         <v>289</v>
       </c>
@@ -10809,7 +12160,7 @@
       </c>
     </row>
     <row r="31" spans="2:22">
-      <c r="B31" s="43"/>
+      <c r="B31" s="44"/>
       <c r="C31" s="17" t="s">
         <v>290</v>
       </c>
@@ -10888,7 +12239,7 @@
       </c>
     </row>
     <row r="32" spans="2:22">
-      <c r="B32" s="43"/>
+      <c r="B32" s="44"/>
       <c r="C32" s="17" t="s">
         <v>291</v>
       </c>
@@ -10951,7 +12302,7 @@
       </c>
     </row>
     <row r="33" spans="2:22">
-      <c r="B33" s="44"/>
+      <c r="B33" s="45"/>
       <c r="C33" s="17" t="s">
         <v>292</v>
       </c>
@@ -11037,7 +12388,7 @@
       <c r="V34" s="23"/>
     </row>
     <row r="35" spans="2:22">
-      <c r="B35" s="33" t="s">
+      <c r="B35" s="34" t="s">
         <v>238</v>
       </c>
       <c r="C35" s="17" t="s">
@@ -11102,7 +12453,7 @@
       </c>
     </row>
     <row r="36" spans="2:22">
-      <c r="B36" s="34"/>
+      <c r="B36" s="35"/>
       <c r="C36" s="17" t="s">
         <v>287</v>
       </c>
@@ -11165,7 +12516,7 @@
       </c>
     </row>
     <row r="37" spans="2:22">
-      <c r="B37" s="34"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="17" t="s">
         <v>288</v>
       </c>
@@ -11228,7 +12579,7 @@
       </c>
     </row>
     <row r="38" spans="2:22">
-      <c r="B38" s="34"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="17" t="s">
         <v>289</v>
       </c>
@@ -11291,7 +12642,7 @@
       </c>
     </row>
     <row r="39" spans="2:22">
-      <c r="B39" s="34"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="17" t="s">
         <v>290</v>
       </c>
@@ -11370,7 +12721,7 @@
       </c>
     </row>
     <row r="40" spans="2:22">
-      <c r="B40" s="34"/>
+      <c r="B40" s="35"/>
       <c r="C40" s="17" t="s">
         <v>291</v>
       </c>
@@ -11433,7 +12784,7 @@
       </c>
     </row>
     <row r="41" spans="2:22">
-      <c r="B41" s="35"/>
+      <c r="B41" s="36"/>
       <c r="C41" s="17" t="s">
         <v>292</v>
       </c>
@@ -11519,7 +12870,7 @@
       <c r="V42" s="23"/>
     </row>
     <row r="43" spans="2:22">
-      <c r="B43" s="33" t="s">
+      <c r="B43" s="34" t="s">
         <v>244</v>
       </c>
       <c r="C43" s="17" t="s">
@@ -11584,7 +12935,7 @@
       </c>
     </row>
     <row r="44" spans="2:22">
-      <c r="B44" s="34"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="17" t="s">
         <v>287</v>
       </c>
@@ -11647,7 +12998,7 @@
       </c>
     </row>
     <row r="45" spans="2:22">
-      <c r="B45" s="34"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="17" t="s">
         <v>288</v>
       </c>
@@ -11710,7 +13061,7 @@
       </c>
     </row>
     <row r="46" spans="2:22">
-      <c r="B46" s="34"/>
+      <c r="B46" s="35"/>
       <c r="C46" s="17" t="s">
         <v>289</v>
       </c>
@@ -11773,7 +13124,7 @@
       </c>
     </row>
     <row r="47" spans="2:22">
-      <c r="B47" s="34"/>
+      <c r="B47" s="35"/>
       <c r="C47" s="17" t="s">
         <v>290</v>
       </c>
@@ -11852,7 +13203,7 @@
       </c>
     </row>
     <row r="48" spans="2:22">
-      <c r="B48" s="34"/>
+      <c r="B48" s="35"/>
       <c r="C48" s="17" t="s">
         <v>291</v>
       </c>
@@ -11915,7 +13266,7 @@
       </c>
     </row>
     <row r="49" spans="2:22">
-      <c r="B49" s="35"/>
+      <c r="B49" s="36"/>
       <c r="C49" s="17" t="s">
         <v>292</v>
       </c>
@@ -12001,7 +13352,7 @@
       <c r="V50" s="23"/>
     </row>
     <row r="51" spans="2:22">
-      <c r="B51" s="33" t="s">
+      <c r="B51" s="34" t="s">
         <v>249</v>
       </c>
       <c r="C51" s="17" t="s">
@@ -12066,7 +13417,7 @@
       </c>
     </row>
     <row r="52" spans="2:22">
-      <c r="B52" s="34"/>
+      <c r="B52" s="35"/>
       <c r="C52" s="17" t="s">
         <v>287</v>
       </c>
@@ -12129,7 +13480,7 @@
       </c>
     </row>
     <row r="53" spans="2:22">
-      <c r="B53" s="34"/>
+      <c r="B53" s="35"/>
       <c r="C53" s="17" t="s">
         <v>288</v>
       </c>
@@ -12192,7 +13543,7 @@
       </c>
     </row>
     <row r="54" spans="2:22">
-      <c r="B54" s="34"/>
+      <c r="B54" s="35"/>
       <c r="C54" s="17" t="s">
         <v>289</v>
       </c>
@@ -12255,7 +13606,7 @@
       </c>
     </row>
     <row r="55" spans="2:22">
-      <c r="B55" s="34"/>
+      <c r="B55" s="35"/>
       <c r="C55" s="17" t="s">
         <v>290</v>
       </c>
@@ -12334,7 +13685,7 @@
       </c>
     </row>
     <row r="56" spans="2:22">
-      <c r="B56" s="34"/>
+      <c r="B56" s="35"/>
       <c r="C56" s="17" t="s">
         <v>291</v>
       </c>
@@ -12397,7 +13748,7 @@
       </c>
     </row>
     <row r="57" spans="2:22">
-      <c r="B57" s="35"/>
+      <c r="B57" s="36"/>
       <c r="C57" s="17" t="s">
         <v>292</v>
       </c>
@@ -12483,7 +13834,7 @@
       <c r="V58" s="23"/>
     </row>
     <row r="59" spans="2:22">
-      <c r="B59" s="33" t="s">
+      <c r="B59" s="34" t="s">
         <v>252</v>
       </c>
       <c r="C59" s="17" t="s">
@@ -12548,7 +13899,7 @@
       </c>
     </row>
     <row r="60" spans="2:22">
-      <c r="B60" s="34"/>
+      <c r="B60" s="35"/>
       <c r="C60" s="17" t="s">
         <v>287</v>
       </c>
@@ -12611,7 +13962,7 @@
       </c>
     </row>
     <row r="61" spans="2:22">
-      <c r="B61" s="34"/>
+      <c r="B61" s="35"/>
       <c r="C61" s="17" t="s">
         <v>288</v>
       </c>
@@ -12674,7 +14025,7 @@
       </c>
     </row>
     <row r="62" spans="2:22">
-      <c r="B62" s="34"/>
+      <c r="B62" s="35"/>
       <c r="C62" s="17" t="s">
         <v>289</v>
       </c>
@@ -12737,7 +14088,7 @@
       </c>
     </row>
     <row r="63" spans="2:22">
-      <c r="B63" s="34"/>
+      <c r="B63" s="35"/>
       <c r="C63" s="17" t="s">
         <v>290</v>
       </c>
@@ -12816,7 +14167,7 @@
       </c>
     </row>
     <row r="64" spans="2:22">
-      <c r="B64" s="34"/>
+      <c r="B64" s="35"/>
       <c r="C64" s="17" t="s">
         <v>291</v>
       </c>
@@ -12879,7 +14230,7 @@
       </c>
     </row>
     <row r="65" spans="2:22">
-      <c r="B65" s="35"/>
+      <c r="B65" s="36"/>
       <c r="C65" s="17" t="s">
         <v>292</v>
       </c>
@@ -12982,534 +14333,492 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B7D490-4724-44DB-9756-35EF11163C36}">
-  <dimension ref="A1:G16"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9A7465-24BE-4C63-8078-09731E2BFE20}">
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>244</v>
-      </c>
-      <c r="B2" t="s">
-        <v>337</v>
-      </c>
-      <c r="C2" t="s">
-        <v>354</v>
-      </c>
-      <c r="D2" t="s">
-        <v>242</v>
-      </c>
-      <c r="E2" t="s">
-        <v>242</v>
-      </c>
-      <c r="F2" t="s">
-        <v>229</v>
-      </c>
-      <c r="G2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>369</v>
-      </c>
-      <c r="B3" t="s">
-        <v>338</v>
-      </c>
-      <c r="C3" t="s">
-        <v>355</v>
-      </c>
-      <c r="D3" t="s">
-        <v>247</v>
-      </c>
-      <c r="E3" t="s">
-        <v>248</v>
-      </c>
-      <c r="F3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>370</v>
-      </c>
-      <c r="B4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C4" t="s">
-        <v>356</v>
-      </c>
-      <c r="D4" t="s">
-        <v>247</v>
-      </c>
-      <c r="E4" t="s">
-        <v>248</v>
-      </c>
-      <c r="F4" t="s">
-        <v>229</v>
-      </c>
-      <c r="G4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>371</v>
-      </c>
-      <c r="B5" t="s">
-        <v>340</v>
-      </c>
-      <c r="C5" t="s">
-        <v>357</v>
-      </c>
-      <c r="D5" t="s">
-        <v>247</v>
-      </c>
-      <c r="E5" t="s">
-        <v>248</v>
-      </c>
-      <c r="F5" t="s">
-        <v>229</v>
-      </c>
-      <c r="G5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>372</v>
-      </c>
-      <c r="B6" t="s">
-        <v>341</v>
-      </c>
-      <c r="C6" t="s">
-        <v>358</v>
-      </c>
-      <c r="D6" t="s">
-        <v>247</v>
-      </c>
-      <c r="E6" t="s">
-        <v>247</v>
-      </c>
-      <c r="F6" t="s">
-        <v>229</v>
-      </c>
-      <c r="G6" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>381</v>
-      </c>
-      <c r="B7" t="s">
-        <v>342</v>
-      </c>
-      <c r="C7" t="s">
-        <v>359</v>
-      </c>
-      <c r="D7" t="s">
-        <v>247</v>
-      </c>
-      <c r="E7" t="s">
-        <v>242</v>
-      </c>
-      <c r="F7" t="s">
-        <v>229</v>
-      </c>
-      <c r="G7" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>373</v>
-      </c>
-      <c r="B8" t="s">
-        <v>343</v>
-      </c>
-      <c r="C8" t="s">
-        <v>360</v>
-      </c>
-      <c r="D8" t="s">
-        <v>242</v>
-      </c>
-      <c r="E8" t="s">
-        <v>248</v>
-      </c>
-      <c r="F8" t="s">
-        <v>229</v>
-      </c>
-      <c r="G8" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>374</v>
-      </c>
-      <c r="B9" t="s">
-        <v>344</v>
-      </c>
-      <c r="C9" t="s">
-        <v>361</v>
-      </c>
-      <c r="D9" t="s">
-        <v>247</v>
-      </c>
-      <c r="E9" t="s">
-        <v>248</v>
-      </c>
-      <c r="F9" t="s">
-        <v>229</v>
-      </c>
-      <c r="G9" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>375</v>
-      </c>
-      <c r="B10" t="s">
-        <v>345</v>
-      </c>
-      <c r="C10" t="s">
-        <v>362</v>
-      </c>
-      <c r="D10" t="s">
-        <v>247</v>
-      </c>
-      <c r="E10" t="s">
-        <v>248</v>
-      </c>
-      <c r="F10" t="s">
-        <v>229</v>
-      </c>
-      <c r="G10" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>376</v>
-      </c>
-      <c r="B11" t="s">
-        <v>346</v>
-      </c>
-      <c r="C11" t="s">
-        <v>363</v>
-      </c>
-      <c r="D11" t="s">
-        <v>247</v>
-      </c>
-      <c r="E11" t="s">
-        <v>242</v>
-      </c>
-      <c r="F11" t="s">
-        <v>229</v>
-      </c>
-      <c r="G11" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>377</v>
-      </c>
-      <c r="B12" t="s">
-        <v>347</v>
-      </c>
-      <c r="C12" t="s">
-        <v>364</v>
-      </c>
-      <c r="D12" t="s">
-        <v>247</v>
-      </c>
-      <c r="E12" t="s">
-        <v>242</v>
-      </c>
-      <c r="F12" t="s">
-        <v>229</v>
-      </c>
-      <c r="G12" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>378</v>
-      </c>
-      <c r="B13" t="s">
-        <v>348</v>
-      </c>
-      <c r="C13" t="s">
-        <v>365</v>
-      </c>
-      <c r="D13" t="s">
-        <v>242</v>
-      </c>
-      <c r="E13" t="s">
-        <v>248</v>
-      </c>
-      <c r="F13" t="s">
-        <v>229</v>
-      </c>
-      <c r="G13" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>379</v>
-      </c>
-      <c r="B14" t="s">
-        <v>349</v>
-      </c>
-      <c r="C14" t="s">
-        <v>366</v>
-      </c>
-      <c r="D14" t="s">
-        <v>247</v>
-      </c>
-      <c r="E14" t="s">
-        <v>242</v>
-      </c>
-      <c r="F14" t="s">
-        <v>229</v>
-      </c>
-      <c r="G14" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>252</v>
-      </c>
-      <c r="B15" t="s">
-        <v>350</v>
-      </c>
-      <c r="C15" t="s">
-        <v>367</v>
-      </c>
-      <c r="D15" t="s">
-        <v>248</v>
-      </c>
-      <c r="E15" t="s">
-        <v>248</v>
-      </c>
-      <c r="F15" t="s">
-        <v>229</v>
-      </c>
-      <c r="G15" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>380</v>
-      </c>
-      <c r="B16" t="s">
-        <v>351</v>
-      </c>
-      <c r="C16" t="s">
-        <v>368</v>
-      </c>
-      <c r="D16" t="s">
-        <v>247</v>
-      </c>
-      <c r="E16" t="s">
-        <v>242</v>
-      </c>
-      <c r="F16" t="s">
-        <v>229</v>
-      </c>
-      <c r="G16" t="s">
-        <v>243</v>
-      </c>
+    <row r="1" spans="1:8">
+      <c r="B1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D1" t="s">
+        <v>401</v>
+      </c>
+      <c r="E1" t="s">
+        <v>402</v>
+      </c>
+      <c r="F1" t="s">
+        <v>403</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>404</v>
+      </c>
+      <c r="H1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.44</v>
+      </c>
+      <c r="C2">
+        <v>0.39</v>
+      </c>
+      <c r="D2">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="E2">
+        <f>(B2*1000)/C2</f>
+        <v>1128.2051282051282</v>
+      </c>
+      <c r="F2">
+        <f>D2*E2</f>
+        <v>1.8051282051282052</v>
+      </c>
+      <c r="G2" s="33">
+        <f>F2*1000/1000</f>
+        <v>1.8051282051282052</v>
+      </c>
+      <c r="H2">
+        <f>(G2/B2)*1000</f>
+        <v>4102.5641025641025</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="G3" s="33"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.42</v>
+      </c>
+      <c r="C4">
+        <v>0.37</v>
+      </c>
+      <c r="D4">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="E4">
+        <f>(B4*1000)/C4</f>
+        <v>1135.1351351351352</v>
+      </c>
+      <c r="F4">
+        <f>D4*E4</f>
+        <v>1.8162162162162165</v>
+      </c>
+      <c r="G4" s="33">
+        <f t="shared" ref="G4:G19" si="0">F4*1000/1000</f>
+        <v>1.8162162162162165</v>
+      </c>
+      <c r="H4">
+        <f>(G4/B4)*1000</f>
+        <v>4324.3243243243251</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C5">
+        <v>0.51</v>
+      </c>
+      <c r="D5">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="E5">
+        <f>(B5*1000)/C5</f>
+        <v>1137.2549019607843</v>
+      </c>
+      <c r="F5">
+        <f>D5*E5</f>
+        <v>2.388235294117647</v>
+      </c>
+      <c r="G5" s="33">
+        <f t="shared" si="0"/>
+        <v>2.388235294117647</v>
+      </c>
+      <c r="H5">
+        <f>(G5/B5)*1000</f>
+        <v>4117.6470588235297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.52</v>
+      </c>
+      <c r="C6">
+        <v>0.46</v>
+      </c>
+      <c r="D6">
+        <v>2E-3</v>
+      </c>
+      <c r="E6">
+        <f>(B6*1000)/C6</f>
+        <v>1130.4347826086955</v>
+      </c>
+      <c r="F6">
+        <f>D6*E6</f>
+        <v>2.2608695652173911</v>
+      </c>
+      <c r="G6" s="33">
+        <f t="shared" si="0"/>
+        <v>2.2608695652173911</v>
+      </c>
+      <c r="H6">
+        <f>(G6/B6)*1000</f>
+        <v>4347.8260869565211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.84</v>
+      </c>
+      <c r="C7">
+        <v>0.74</v>
+      </c>
+      <c r="D7">
+        <v>3.0999999999999999E-3</v>
+      </c>
+      <c r="E7">
+        <f>(B7*1000)/C7</f>
+        <v>1135.1351351351352</v>
+      </c>
+      <c r="F7">
+        <f>D7*E7</f>
+        <v>3.5189189189189189</v>
+      </c>
+      <c r="G7" s="33">
+        <f t="shared" si="0"/>
+        <v>3.5189189189189189</v>
+      </c>
+      <c r="H7">
+        <f>(G7/B7)*1000</f>
+        <v>4189.1891891891892</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="G8" s="33"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.65</v>
+      </c>
+      <c r="C9">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D9">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="E9">
+        <f>(B9*1000)/C9</f>
+        <v>1120.6896551724139</v>
+      </c>
+      <c r="F9">
+        <f>D9*E9</f>
+        <v>2.6896551724137931</v>
+      </c>
+      <c r="G9" s="33">
+        <f t="shared" si="0"/>
+        <v>2.6896551724137931</v>
+      </c>
+      <c r="H9">
+        <f>(G9/B9)*1000</f>
+        <v>4137.9310344827591</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C10">
+        <v>1.02</v>
+      </c>
+      <c r="D10">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E10">
+        <f>(B10*1000)/C10</f>
+        <v>1127.4509803921569</v>
+      </c>
+      <c r="F10">
+        <f>D10*E10</f>
+        <v>4.5098039215686274</v>
+      </c>
+      <c r="G10" s="33">
+        <f t="shared" si="0"/>
+        <v>4.5098039215686274</v>
+      </c>
+      <c r="H10">
+        <f>(G10/B10)*1000</f>
+        <v>3921.5686274509808</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0.69</v>
+      </c>
+      <c r="C11">
+        <v>0.61</v>
+      </c>
+      <c r="D11">
+        <v>2.3E-3</v>
+      </c>
+      <c r="E11">
+        <f>(B11*1000)/C11</f>
+        <v>1131.1475409836066</v>
+      </c>
+      <c r="F11">
+        <f>D11*E11</f>
+        <v>2.6016393442622952</v>
+      </c>
+      <c r="G11" s="33">
+        <f t="shared" si="0"/>
+        <v>2.6016393442622952</v>
+      </c>
+      <c r="H11">
+        <f>(G11/B11)*1000</f>
+        <v>3770.4918032786886</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0.7</v>
+      </c>
+      <c r="C12">
+        <v>0.62</v>
+      </c>
+      <c r="D12">
+        <v>2E-3</v>
+      </c>
+      <c r="E12">
+        <f>(B12*1000)/C12</f>
+        <v>1129.0322580645161</v>
+      </c>
+      <c r="F12">
+        <f>D12*E12</f>
+        <v>2.258064516129032</v>
+      </c>
+      <c r="G12" s="33">
+        <f t="shared" si="0"/>
+        <v>2.258064516129032</v>
+      </c>
+      <c r="H12">
+        <f>(G12/B12)*1000</f>
+        <v>3225.8064516129029</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0.54</v>
+      </c>
+      <c r="C13">
+        <v>0.48</v>
+      </c>
+      <c r="D13">
+        <v>1.8E-3</v>
+      </c>
+      <c r="E13">
+        <f>(B13*1000)/C13</f>
+        <v>1125</v>
+      </c>
+      <c r="F13">
+        <f>D13*E13</f>
+        <v>2.0249999999999999</v>
+      </c>
+      <c r="G13" s="33">
+        <f t="shared" si="0"/>
+        <v>2.0249999999999999</v>
+      </c>
+      <c r="H13">
+        <f>(G13/B13)*1000</f>
+        <v>3749.9999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="G14" s="33"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C15">
+        <v>0.49</v>
+      </c>
+      <c r="D15">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="E15">
+        <f>(B15*1000)/C15</f>
+        <v>1142.8571428571429</v>
+      </c>
+      <c r="F15">
+        <f>D15*E15</f>
+        <v>1.9428571428571428</v>
+      </c>
+      <c r="G15" s="33">
+        <f t="shared" si="0"/>
+        <v>1.9428571428571428</v>
+      </c>
+      <c r="H15">
+        <f>(G15/B15)*1000</f>
+        <v>3469.3877551020405</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="G16" s="33"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0.71</v>
+      </c>
+      <c r="C17">
+        <v>0.63</v>
+      </c>
+      <c r="D17">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="E17">
+        <f>(B17*1000)/C17</f>
+        <v>1126.984126984127</v>
+      </c>
+      <c r="F17">
+        <f>D17*E17</f>
+        <v>2.4793650793650794</v>
+      </c>
+      <c r="G17" s="33">
+        <f t="shared" si="0"/>
+        <v>2.4793650793650794</v>
+      </c>
+      <c r="H17">
+        <f>(G17/B17)*1000</f>
+        <v>3492.0634920634925</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1.17</v>
+      </c>
+      <c r="C18">
+        <v>1.03</v>
+      </c>
+      <c r="D18">
+        <v>3.7000000000000002E-3</v>
+      </c>
+      <c r="E18">
+        <f>(B18*1000)/C18</f>
+        <v>1135.9223300970873</v>
+      </c>
+      <c r="F18">
+        <f>D18*E18</f>
+        <v>4.2029126213592232</v>
+      </c>
+      <c r="G18" s="33">
+        <f t="shared" si="0"/>
+        <v>4.2029126213592232</v>
+      </c>
+      <c r="H18">
+        <f>(G18/B18)*1000</f>
+        <v>3592.2330097087379</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>2.88</v>
+      </c>
+      <c r="C19">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="D19">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="E19">
+        <f>(B19*1000)/C19</f>
+        <v>1129.4117647058824</v>
+      </c>
+      <c r="F19">
+        <f>D19*E19</f>
+        <v>11.181176470588237</v>
+      </c>
+      <c r="G19" s="33">
+        <f t="shared" si="0"/>
+        <v>11.181176470588237</v>
+      </c>
+      <c r="H19">
+        <f>(G19/B19)*1000</f>
+        <v>3882.3529411764716</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="G20" s="33"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="G21" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33AA0F0-47E1-4AC0-A88E-CD4E07267161}">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="35.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>335</v>
-      </c>
-      <c r="B1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>337</v>
-      </c>
-      <c r="B2">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>338</v>
-      </c>
-      <c r="B3">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>339</v>
-      </c>
-      <c r="B4">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>340</v>
-      </c>
-      <c r="B5">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>341</v>
-      </c>
-      <c r="B6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>342</v>
-      </c>
-      <c r="B7">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>343</v>
-      </c>
-      <c r="B8">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>344</v>
-      </c>
-      <c r="B9">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>345</v>
-      </c>
-      <c r="B10">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>346</v>
-      </c>
-      <c r="B11">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>347</v>
-      </c>
-      <c r="B12">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>348</v>
-      </c>
-      <c r="B13">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>349</v>
-      </c>
-      <c r="B14">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>350</v>
-      </c>
-      <c r="B15">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>351</v>
-      </c>
-      <c r="B16">
-        <v>151</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13523,6 +14832,19 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0577e6a0-5f74-4659-a81a-c7bdc984432d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FF634CA3F5682C418397C6E4414BCDE3" ma:contentTypeVersion="19" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="dcc84226a5c9737fccd97eea407b26d6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0577e6a0-5f74-4659-a81a-c7bdc984432d" xmlns:ns3="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="412c1c7c3b81559b33b856787a43d0a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -13788,19 +15110,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0577e6a0-5f74-4659-a81a-c7bdc984432d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD6878A0-F687-4E6D-A191-8D8ADCEF84BD}">
   <ds:schemaRefs>
@@ -13810,6 +15119,24 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7FDE463-4D3F-41EC-839E-DA16C78214B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="0577e6a0-5f74-4659-a81a-c7bdc984432d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1A97AFE-C266-46C6-A1B3-B4280223A46E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13827,22 +15154,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7FDE463-4D3F-41EC-839E-DA16C78214B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="0577e6a0-5f74-4659-a81a-c7bdc984432d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update vignette showing sensitivity analysis using "Base functions.R"
</commit_message>
<xml_diff>
--- a/data/TWP emission data_IDIADA_v01_andSIML.xlsx
+++ b/data/TWP emission data_IDIADA_v01_andSIML.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quikj\rivm.nl\LEON-Tyres - WP3 Microplastics\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rivmnl-my.sharepoint.com/personal/joris_quik_rivm_nl/Documents/Git projects/tyre-friction-abrassion-emission_2024/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881749E5-F2BB-4584-8094-F28CF42164A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{881749E5-F2BB-4584-8094-F28CF42164A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4F3387D-B5D0-418D-9864-C8D26C60C6C0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="9" xr2:uid="{1B08EC6D-E4F6-452D-BA0B-C8BBC214CF8F}"/>
+    <workbookView xWindow="13410" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{1B08EC6D-E4F6-452D-BA0B-C8BBC214CF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="8" r:id="rId1"/>
@@ -33,8 +33,6 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Abrasion_ADAC!$B$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Abrasion_ADAC!$B$2:$B$16</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Abrasion_ADAC!$B$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Abrasion_ADAC!$B$2:$B$16</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1513,9 +1511,6 @@
     <t>MMoWStr3</t>
   </si>
   <si>
-    <t>MMoWStr4</t>
-  </si>
-  <si>
     <t>Abrasion rate (mg/km)</t>
   </si>
   <si>
@@ -1541,6 +1536,9 @@
   </si>
   <si>
     <t>Friction per km (kJ/km)</t>
+  </si>
+  <si>
+    <t>MMoWB1</t>
   </si>
 </sst>
 </file>
@@ -1990,7 +1988,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2000,7 +1998,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{8C34953D-F100-4CEF-B70A-5C3E49BCC665}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>Abrasion rate (mg/km)</cx:v>
             </cx:txData>
           </cx:tx>
@@ -2767,8 +2765,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3733800" y="323850"/>
-              <a:ext cx="2164080" cy="2743200"/>
+              <a:off x="3733800" y="320040"/>
+              <a:ext cx="2162175" cy="2714625"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3350,7 +3348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33AA0F0-47E1-4AC0-A88E-CD4E07267161}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18:G22"/>
     </sheetView>
   </sheetViews>
@@ -3361,10 +3359,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6250,9 +6248,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04A54C1-E4DA-444B-8C3A-50F2DC127EAA}">
   <dimension ref="A1:L105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -10064,7 +10062,7 @@
         <v>389</v>
       </c>
       <c r="D101" s="32" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
       <c r="E101" s="32" t="s">
         <v>120</v>
@@ -10204,7 +10202,7 @@
         <v>389</v>
       </c>
       <c r="D105" s="32" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
       <c r="E105" s="32" t="s">
         <v>120</v>
@@ -14345,25 +14343,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C1" t="s">
         <v>399</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>400</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>401</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>402</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="33" t="s">
         <v>403</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="H1" t="s">
         <v>404</v>
-      </c>
-      <c r="H1" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -14823,28 +14821,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0577e6a0-5f74-4659-a81a-c7bdc984432d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FF634CA3F5682C418397C6E4414BCDE3" ma:contentTypeVersion="19" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="dcc84226a5c9737fccd97eea407b26d6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0577e6a0-5f74-4659-a81a-c7bdc984432d" xmlns:ns3="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="412c1c7c3b81559b33b856787a43d0a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15110,10 +15086,44 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0577e6a0-5f74-4659-a81a-c7bdc984432d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD6878A0-F687-4E6D-A191-8D8ADCEF84BD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1A97AFE-C266-46C6-A1B3-B4280223A46E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="0577e6a0-5f74-4659-a81a-c7bdc984432d"/>
+    <ds:schemaRef ds:uri="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -15137,21 +15147,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1A97AFE-C266-46C6-A1B3-B4280223A46E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD6878A0-F687-4E6D-A191-8D8ADCEF84BD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="0577e6a0-5f74-4659-a81a-c7bdc984432d"/>
-    <ds:schemaRef ds:uri="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>